<commit_message>
Updated to work with new GUI and Network Code
</commit_message>
<xml_diff>
--- a/comms.xlsx
+++ b/comms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\games\util-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30293BDA-5965-49A4-8D91-872E56C044A4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A873305E-9F1E-4E05-9812-E767EB4A907D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{AF0E65F2-BC31-479C-9376-84253AE83124}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7980" xr2:uid="{AF0E65F2-BC31-479C-9376-84253AE83124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Server</t>
   </si>
@@ -129,6 +129,48 @@
   </si>
   <si>
     <t>&lt;- 'connectionmanager-connect'</t>
+  </si>
+  <si>
+    <t>SERVER</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+  </si>
+  <si>
+    <t>open call</t>
+  </si>
+  <si>
+    <t>watch server side object properties</t>
+  </si>
+  <si>
+    <t>send open event to client</t>
+  </si>
+  <si>
+    <t>watch client side properties</t>
+  </si>
+  <si>
+    <t>open gui element</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>property update</t>
+  </si>
+  <si>
+    <t>send event to client</t>
+  </si>
+  <si>
+    <t>update value on DOM</t>
+  </si>
+  <si>
+    <t>dom property change (user event)</t>
+  </si>
+  <si>
+    <t>send event to server</t>
+  </si>
+  <si>
+    <t>update property on object</t>
   </si>
 </sst>
 </file>
@@ -164,13 +206,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -487,97 +532,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CBE335-41F6-4CA2-8EE7-BC7DBD273F97}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>